<commit_message>
Pio's ERA operativo Abril-Diciembre 2025
</commit_message>
<xml_diff>
--- a/AA - Calendario de Turnos(version Agosto-Diciembre 2024).xlsx
+++ b/AA - Calendario de Turnos(version Agosto-Diciembre 2024).xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I165"/>
+  <dimension ref="A1:I153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,12 +543,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>Boettiger</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>Pio</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Alvo</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -671,7 +671,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Boettiger</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -712,7 +712,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Loch</t>
+          <t>Boettiger</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -753,7 +753,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Rubio</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -794,7 +794,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Contreras</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -830,12 +830,12 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Alvo</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Cisternas</t>
+          <t>Contreras</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -958,7 +958,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Pio</t>
+          <t>Cisternas</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1040,7 +1040,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Alvo</t>
+          <t>Pio</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1117,12 +1117,12 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Boettiger</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Boettiger</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1245,7 +1245,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Loch</t>
+          <t>Boettiger</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1286,7 +1286,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Rubio</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1327,7 +1327,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Contreras</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1368,7 +1368,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Cisternas</t>
+          <t>Contreras</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1404,12 +1404,12 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Loch</t>
+          <t>Pio</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Pio</t>
+          <t>Cisternas</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1573,7 +1573,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Alvo</t>
+          <t>Pio</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -1614,7 +1614,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Boettiger</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -1655,7 +1655,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Loch</t>
+          <t>Boettiger</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -1691,12 +1691,12 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Rubio</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Rubio</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -1819,7 +1819,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Contreras</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -1860,7 +1860,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Cisternas</t>
+          <t>Contreras</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -1901,7 +1901,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Pio</t>
+          <t>Cisternas</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -1983,7 +1983,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Alvo</t>
+          <t>Pio</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -2106,7 +2106,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Boettiger</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -2147,7 +2147,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Loch</t>
+          <t>Boettiger</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -2188,7 +2188,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Rubio</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -2229,7 +2229,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Contreras</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -2265,12 +2265,12 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Pio</t>
+          <t>Boettiger</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Cisternas</t>
+          <t>Contreras</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -2393,7 +2393,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Pio</t>
+          <t>Cisternas</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -2552,12 +2552,12 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Alvo</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Alvo</t>
+          <t>Pio</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -2680,7 +2680,7 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Boettiger</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
@@ -2721,7 +2721,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Loch</t>
+          <t>Boettiger</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
@@ -2762,7 +2762,7 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>Rubio</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
@@ -2803,7 +2803,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Contreras</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
@@ -2839,12 +2839,12 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Boettiger</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Cisternas</t>
+          <t>Contreras</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
@@ -2967,7 +2967,7 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>Pio</t>
+          <t>Cisternas</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
@@ -3049,7 +3049,7 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Alvo</t>
+          <t>Pio</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
@@ -3090,7 +3090,7 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>Boettiger</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
@@ -3126,12 +3126,12 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Loch</t>
+          <t>Pio</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Loch</t>
+          <t>Boettiger</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
@@ -3254,7 +3254,7 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Rubio</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
@@ -3295,7 +3295,7 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Contreras</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
@@ -3336,7 +3336,7 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>Cisternas</t>
+          <t>Contreras</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
@@ -3377,7 +3377,7 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>Pio</t>
+          <t>Cisternas</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
@@ -3413,7 +3413,7 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Rubio</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
@@ -3541,7 +3541,7 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>Alvo</t>
+          <t>Pio</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
@@ -3582,7 +3582,7 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>Boettiger</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
@@ -3623,7 +3623,7 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Loch</t>
+          <t>Boettiger</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
@@ -3664,7 +3664,7 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>Rubio</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
@@ -3705,7 +3705,7 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>Contreras</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
@@ -3828,7 +3828,7 @@
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>Cisternas</t>
+          <t>Recluta1</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
@@ -3869,7 +3869,7 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>Pio</t>
+          <t>Contreras</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
@@ -3910,7 +3910,7 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>Recluta1</t>
+          <t>Cisternas</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
@@ -3951,7 +3951,7 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>Alvo</t>
+          <t>Pio</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
@@ -3987,12 +3987,12 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Pio</t>
+          <t>Boettiger</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>Boettiger</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
@@ -4023,17 +4023,17 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Pio</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Pio</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>Pio</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="H88" t="inlineStr">
@@ -4064,17 +4064,17 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Alvo</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Alvo</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>Alvo</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="H89" t="inlineStr">
@@ -4115,7 +4115,7 @@
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>Loch</t>
+          <t>Boettiger</t>
         </is>
       </c>
       <c r="H90" t="inlineStr">
@@ -4156,7 +4156,7 @@
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>Rubio</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="H91" t="inlineStr">
@@ -4197,7 +4197,7 @@
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>Recluta1</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="H92" t="inlineStr">
@@ -4402,7 +4402,7 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>Contreras</t>
+          <t>Recluta1</t>
         </is>
       </c>
       <c r="H97" t="inlineStr">
@@ -4443,7 +4443,7 @@
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>Cisternas</t>
+          <t>Contreras</t>
         </is>
       </c>
       <c r="H98" t="inlineStr">
@@ -4484,7 +4484,7 @@
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>Pio</t>
+          <t>Cisternas</t>
         </is>
       </c>
       <c r="H99" t="inlineStr">
@@ -4525,7 +4525,7 @@
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>Alvo</t>
+          <t>Pio</t>
         </is>
       </c>
       <c r="H100" t="inlineStr">
@@ -4561,12 +4561,12 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
+          <t>Loch</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
           <t>Alvo</t>
-        </is>
-      </c>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>Boettiger</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">
@@ -4597,17 +4597,17 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Boettiger</t>
+          <t>Recluta1</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>Boettiger</t>
+          <t>Recluta1</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>Boettiger</t>
+          <t>Recluta1</t>
         </is>
       </c>
       <c r="H102" t="inlineStr">
@@ -4638,17 +4638,17 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>Loch</t>
+          <t>Gomez</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>Loch</t>
+          <t>Gomez</t>
         </is>
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>Loch</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="H103" t="inlineStr">
@@ -4689,7 +4689,7 @@
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>Loch</t>
+          <t>Boettiger</t>
         </is>
       </c>
       <c r="H104" t="inlineStr">
@@ -4730,7 +4730,7 @@
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>Rubio</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="H105" t="inlineStr">
@@ -4771,7 +4771,7 @@
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>Recluta1</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="H106" t="inlineStr">
@@ -4812,7 +4812,7 @@
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>Contreras</t>
+          <t>Recluta1</t>
         </is>
       </c>
       <c r="H107" t="inlineStr">
@@ -4848,12 +4848,12 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>Boettiger</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>Cisternas</t>
+          <t>Contreras</t>
         </is>
       </c>
       <c r="H108" t="inlineStr">
@@ -4884,17 +4884,17 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>Rubio</t>
+          <t>Bravo</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>Rubio</t>
+          <t>Bravo</t>
         </is>
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>Rubio</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="H109" t="inlineStr">
@@ -4925,17 +4925,17 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Recluta1</t>
+          <t>Iñiguez</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>Recluta1</t>
+          <t>Iñiguez</t>
         </is>
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>Recluta1</t>
+          <t>Boettiger</t>
         </is>
       </c>
       <c r="H110" t="inlineStr">
@@ -4976,7 +4976,7 @@
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>Pio</t>
+          <t>Cisternas</t>
         </is>
       </c>
       <c r="H111" t="inlineStr">
@@ -5017,7 +5017,7 @@
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>Alvo</t>
+          <t>Pio</t>
         </is>
       </c>
       <c r="H112" t="inlineStr">
@@ -5058,7 +5058,7 @@
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>Boettiger</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="H113" t="inlineStr">
@@ -5099,7 +5099,7 @@
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>Loch</t>
+          <t>Boettiger</t>
         </is>
       </c>
       <c r="H114" t="inlineStr">
@@ -5135,12 +5135,12 @@
       </c>
       <c r="F115" t="inlineStr">
         <is>
+          <t>Pio</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
           <t>Loch</t>
-        </is>
-      </c>
-      <c r="G115" t="inlineStr">
-        <is>
-          <t>Rubio</t>
         </is>
       </c>
       <c r="H115" t="inlineStr">
@@ -5171,17 +5171,17 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>Gomez</t>
+          <t>Breinbauer</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>Gomez</t>
+          <t>Breinbauer</t>
         </is>
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>Rubio</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="H116" t="inlineStr">
@@ -5212,17 +5212,17 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>Bravo</t>
+          <t>Arredondo</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>Bravo</t>
+          <t>Arredondo</t>
         </is>
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>Loch</t>
+          <t>Pio</t>
         </is>
       </c>
       <c r="H117" t="inlineStr">
@@ -5263,7 +5263,7 @@
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>Recluta1</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="H118" t="inlineStr">
@@ -5304,7 +5304,7 @@
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>Contreras</t>
+          <t>Recluta1</t>
         </is>
       </c>
       <c r="H119" t="inlineStr">
@@ -5345,7 +5345,7 @@
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>Cisternas</t>
+          <t>Contreras</t>
         </is>
       </c>
       <c r="H120" t="inlineStr">
@@ -5386,7 +5386,7 @@
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>Pio</t>
+          <t>Cisternas</t>
         </is>
       </c>
       <c r="H121" t="inlineStr">
@@ -5422,12 +5422,12 @@
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>Rubio</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>Alvo</t>
+          <t>Pio</t>
         </is>
       </c>
       <c r="H122" t="inlineStr">
@@ -5458,17 +5458,17 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>Iñiguez</t>
+          <t>Carrasco</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>Iñiguez</t>
+          <t>Carrasco</t>
         </is>
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>Boettiger</t>
+          <t>Recluta1</t>
         </is>
       </c>
       <c r="H123" t="inlineStr">
@@ -5499,17 +5499,17 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>Breinbauer</t>
+          <t>Culaciati</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>Breinbauer</t>
+          <t>Culaciati</t>
         </is>
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>Alvo</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="H124" t="inlineStr">
@@ -5550,7 +5550,7 @@
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>Boettiger</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="H125" t="inlineStr">
@@ -5591,7 +5591,7 @@
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>Loch</t>
+          <t>Boettiger</t>
         </is>
       </c>
       <c r="H126" t="inlineStr">
@@ -5632,7 +5632,7 @@
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>Rubio</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="H127" t="inlineStr">
@@ -5673,7 +5673,7 @@
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>Recluta1</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="H128" t="inlineStr">
@@ -5714,7 +5714,7 @@
       </c>
       <c r="G129" t="inlineStr">
         <is>
-          <t>Contreras</t>
+          <t>Recluta1</t>
         </is>
       </c>
       <c r="H129" t="inlineStr">
@@ -5745,17 +5745,17 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>Arredondo</t>
+          <t>Contreras</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>Arredondo</t>
+          <t>Contreras</t>
         </is>
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>Pio</t>
+          <t>Contreras</t>
         </is>
       </c>
       <c r="H130" t="inlineStr">
@@ -5786,17 +5786,17 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>Carrasco</t>
+          <t>Cisternas</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>Carrasco</t>
+          <t>Cisternas</t>
         </is>
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>Recluta1</t>
+          <t>Cisternas</t>
         </is>
       </c>
       <c r="H131" t="inlineStr">
@@ -5837,7 +5837,7 @@
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>Cisternas</t>
+          <t>Contreras</t>
         </is>
       </c>
       <c r="H132" t="inlineStr">
@@ -5878,7 +5878,7 @@
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>Pio</t>
+          <t>Cisternas</t>
         </is>
       </c>
       <c r="H133" t="inlineStr">
@@ -5919,7 +5919,7 @@
       </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>Alvo</t>
+          <t>Pio</t>
         </is>
       </c>
       <c r="H134" t="inlineStr">
@@ -5960,7 +5960,7 @@
       </c>
       <c r="G135" t="inlineStr">
         <is>
-          <t>Boettiger</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="H135" t="inlineStr">
@@ -5996,12 +5996,12 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>Pio</t>
+          <t>Boettiger</t>
         </is>
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>Loch</t>
+          <t>Boettiger</t>
         </is>
       </c>
       <c r="H136" t="inlineStr">
@@ -6032,17 +6032,17 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>Culaciati</t>
+          <t>Pio</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>Culaciati</t>
+          <t>Pio</t>
         </is>
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>Rubio</t>
+          <t>Pio</t>
         </is>
       </c>
       <c r="H137" t="inlineStr">
@@ -6073,17 +6073,17 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>Contreras</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>Contreras</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="G138" t="inlineStr">
         <is>
-          <t>Contreras</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="H138" t="inlineStr">
@@ -6124,7 +6124,7 @@
       </c>
       <c r="G139" t="inlineStr">
         <is>
-          <t>Rubio</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="H139" t="inlineStr">
@@ -6165,7 +6165,7 @@
       </c>
       <c r="G140" t="inlineStr">
         <is>
-          <t>Recluta1</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="H140" t="inlineStr">
@@ -6206,7 +6206,7 @@
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>Contreras</t>
+          <t>Recluta1</t>
         </is>
       </c>
       <c r="H141" t="inlineStr">
@@ -6247,7 +6247,7 @@
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>Cisternas</t>
+          <t>Contreras</t>
         </is>
       </c>
       <c r="H142" t="inlineStr">
@@ -6283,12 +6283,12 @@
       </c>
       <c r="F143" t="inlineStr">
         <is>
-          <t>Alvo</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>Pio</t>
+          <t>Cisternas</t>
         </is>
       </c>
       <c r="H143" t="inlineStr">
@@ -6319,17 +6319,17 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>Cisternas</t>
+          <t>Boettiger</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
         <is>
-          <t>Cisternas</t>
+          <t>Boettiger</t>
         </is>
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>Cisternas</t>
+          <t>Boettiger</t>
         </is>
       </c>
       <c r="H144" t="inlineStr">
@@ -6360,17 +6360,17 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>Pio</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
         <is>
-          <t>Pio</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="G145" t="inlineStr">
         <is>
-          <t>Pio</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="H145" t="inlineStr">
@@ -6411,7 +6411,7 @@
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>Alvo</t>
+          <t>Pio</t>
         </is>
       </c>
       <c r="H146" t="inlineStr">
@@ -6452,7 +6452,7 @@
       </c>
       <c r="G147" t="inlineStr">
         <is>
-          <t>Boettiger</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="H147" t="inlineStr">
@@ -6534,7 +6534,7 @@
       </c>
       <c r="G149" t="inlineStr">
         <is>
-          <t>Loch</t>
+          <t>Boettiger</t>
         </is>
       </c>
       <c r="H149" t="inlineStr">
@@ -6570,12 +6570,12 @@
       </c>
       <c r="F150" t="inlineStr">
         <is>
-          <t>Boettiger</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>Rubio</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="H150" t="inlineStr">
@@ -6606,17 +6606,17 @@
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>Alvo</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
         <is>
-          <t>Alvo</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>Alvo</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="H151" t="inlineStr">
@@ -6647,17 +6647,17 @@
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>Boettiger</t>
+          <t>Recluta1</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
         <is>
-          <t>Boettiger</t>
+          <t>Recluta1</t>
         </is>
       </c>
       <c r="G152" t="inlineStr">
         <is>
-          <t>Boettiger</t>
+          <t>Recluta1</t>
         </is>
       </c>
       <c r="H152" t="inlineStr">
@@ -6698,7 +6698,7 @@
       </c>
       <c r="G153" t="inlineStr">
         <is>
-          <t>Recluta1</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="H153" t="inlineStr">
@@ -6707,498 +6707,6 @@
         </is>
       </c>
       <c r="I153" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-    </row>
-    <row r="154">
-      <c r="A154" t="n">
-        <v>2024</v>
-      </c>
-      <c r="B154" t="n">
-        <v>12</v>
-      </c>
-      <c r="C154" t="n">
-        <v>31</v>
-      </c>
-      <c r="D154" t="inlineStr">
-        <is>
-          <t>Martes</t>
-        </is>
-      </c>
-      <c r="E154" t="inlineStr">
-        <is>
-          <t>Iñiguez</t>
-        </is>
-      </c>
-      <c r="F154" t="inlineStr">
-        <is>
-          <t>Contreras</t>
-        </is>
-      </c>
-      <c r="G154" t="inlineStr">
-        <is>
-          <t>Contreras</t>
-        </is>
-      </c>
-      <c r="H154" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> - </t>
-        </is>
-      </c>
-      <c r="I154" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-    </row>
-    <row r="155">
-      <c r="A155" t="n">
-        <v>2025</v>
-      </c>
-      <c r="B155" t="n">
-        <v>1</v>
-      </c>
-      <c r="C155" t="n">
-        <v>1</v>
-      </c>
-      <c r="D155" t="inlineStr">
-        <is>
-          <t>Feriado o Especial</t>
-        </is>
-      </c>
-      <c r="E155" t="inlineStr">
-        <is>
-          <t>Sin asignar</t>
-        </is>
-      </c>
-      <c r="F155" t="inlineStr">
-        <is>
-          <t>Sin asignar</t>
-        </is>
-      </c>
-      <c r="G155" t="inlineStr">
-        <is>
-          <t>Feriado o Especial</t>
-        </is>
-      </c>
-      <c r="H155" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> - </t>
-        </is>
-      </c>
-      <c r="I155" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156" t="n">
-        <v>2025</v>
-      </c>
-      <c r="B156" t="n">
-        <v>1</v>
-      </c>
-      <c r="C156" t="n">
-        <v>2</v>
-      </c>
-      <c r="D156" t="inlineStr">
-        <is>
-          <t>Jueves</t>
-        </is>
-      </c>
-      <c r="E156" t="inlineStr">
-        <is>
-          <t>Bravo</t>
-        </is>
-      </c>
-      <c r="F156" t="inlineStr">
-        <is>
-          <t>Culaciati</t>
-        </is>
-      </c>
-      <c r="G156" t="inlineStr">
-        <is>
-          <t>Cisternas</t>
-        </is>
-      </c>
-      <c r="H156" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> - </t>
-        </is>
-      </c>
-      <c r="I156" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-    </row>
-    <row r="157">
-      <c r="A157" t="n">
-        <v>2025</v>
-      </c>
-      <c r="B157" t="n">
-        <v>1</v>
-      </c>
-      <c r="C157" t="n">
-        <v>3</v>
-      </c>
-      <c r="D157" t="inlineStr">
-        <is>
-          <t>Viernes</t>
-        </is>
-      </c>
-      <c r="E157" t="inlineStr">
-        <is>
-          <t>Breinbauer</t>
-        </is>
-      </c>
-      <c r="F157" t="inlineStr">
-        <is>
-          <t>Loch</t>
-        </is>
-      </c>
-      <c r="G157" t="inlineStr">
-        <is>
-          <t>Pio</t>
-        </is>
-      </c>
-      <c r="H157" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> - </t>
-        </is>
-      </c>
-      <c r="I157" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-    </row>
-    <row r="158">
-      <c r="A158" t="n">
-        <v>2025</v>
-      </c>
-      <c r="B158" t="n">
-        <v>1</v>
-      </c>
-      <c r="C158" t="n">
-        <v>4</v>
-      </c>
-      <c r="D158" t="inlineStr">
-        <is>
-          <t>Sábado</t>
-        </is>
-      </c>
-      <c r="E158" t="inlineStr">
-        <is>
-          <t>Loch</t>
-        </is>
-      </c>
-      <c r="F158" t="inlineStr">
-        <is>
-          <t>Loch</t>
-        </is>
-      </c>
-      <c r="G158" t="inlineStr">
-        <is>
-          <t>Loch</t>
-        </is>
-      </c>
-      <c r="H158" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> - </t>
-        </is>
-      </c>
-      <c r="I158" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-    </row>
-    <row r="159">
-      <c r="A159" t="n">
-        <v>2025</v>
-      </c>
-      <c r="B159" t="n">
-        <v>1</v>
-      </c>
-      <c r="C159" t="n">
-        <v>5</v>
-      </c>
-      <c r="D159" t="inlineStr">
-        <is>
-          <t>Domingo</t>
-        </is>
-      </c>
-      <c r="E159" t="inlineStr">
-        <is>
-          <t>Rubio</t>
-        </is>
-      </c>
-      <c r="F159" t="inlineStr">
-        <is>
-          <t>Rubio</t>
-        </is>
-      </c>
-      <c r="G159" t="inlineStr">
-        <is>
-          <t>Rubio</t>
-        </is>
-      </c>
-      <c r="H159" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> - </t>
-        </is>
-      </c>
-      <c r="I159" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-    </row>
-    <row r="160">
-      <c r="A160" t="n">
-        <v>2025</v>
-      </c>
-      <c r="B160" t="n">
-        <v>1</v>
-      </c>
-      <c r="C160" t="n">
-        <v>6</v>
-      </c>
-      <c r="D160" t="inlineStr">
-        <is>
-          <t>Lunes</t>
-        </is>
-      </c>
-      <c r="E160" t="inlineStr">
-        <is>
-          <t>Gomez</t>
-        </is>
-      </c>
-      <c r="F160" t="inlineStr">
-        <is>
-          <t>Cisternas</t>
-        </is>
-      </c>
-      <c r="G160" t="inlineStr">
-        <is>
-          <t>Alvo</t>
-        </is>
-      </c>
-      <c r="H160" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> - </t>
-        </is>
-      </c>
-      <c r="I160" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161" t="n">
-        <v>2025</v>
-      </c>
-      <c r="B161" t="n">
-        <v>1</v>
-      </c>
-      <c r="C161" t="n">
-        <v>7</v>
-      </c>
-      <c r="D161" t="inlineStr">
-        <is>
-          <t>Martes</t>
-        </is>
-      </c>
-      <c r="E161" t="inlineStr">
-        <is>
-          <t>Iñiguez</t>
-        </is>
-      </c>
-      <c r="F161" t="inlineStr">
-        <is>
-          <t>Contreras</t>
-        </is>
-      </c>
-      <c r="G161" t="inlineStr">
-        <is>
-          <t>Boettiger</t>
-        </is>
-      </c>
-      <c r="H161" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> - </t>
-        </is>
-      </c>
-      <c r="I161" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-    </row>
-    <row r="162">
-      <c r="A162" t="n">
-        <v>2025</v>
-      </c>
-      <c r="B162" t="n">
-        <v>1</v>
-      </c>
-      <c r="C162" t="n">
-        <v>8</v>
-      </c>
-      <c r="D162" t="inlineStr">
-        <is>
-          <t>Miércoles</t>
-        </is>
-      </c>
-      <c r="E162" t="inlineStr">
-        <is>
-          <t>Arredondo</t>
-        </is>
-      </c>
-      <c r="F162" t="inlineStr">
-        <is>
-          <t>Carrasco</t>
-        </is>
-      </c>
-      <c r="G162" t="inlineStr">
-        <is>
-          <t>Loch</t>
-        </is>
-      </c>
-      <c r="H162" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> - </t>
-        </is>
-      </c>
-      <c r="I162" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163" t="n">
-        <v>2025</v>
-      </c>
-      <c r="B163" t="n">
-        <v>1</v>
-      </c>
-      <c r="C163" t="n">
-        <v>9</v>
-      </c>
-      <c r="D163" t="inlineStr">
-        <is>
-          <t>Jueves</t>
-        </is>
-      </c>
-      <c r="E163" t="inlineStr">
-        <is>
-          <t>Bravo</t>
-        </is>
-      </c>
-      <c r="F163" t="inlineStr">
-        <is>
-          <t>Culaciati</t>
-        </is>
-      </c>
-      <c r="G163" t="inlineStr">
-        <is>
-          <t>Rubio</t>
-        </is>
-      </c>
-      <c r="H163" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> - </t>
-        </is>
-      </c>
-      <c r="I163" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-    </row>
-    <row r="164">
-      <c r="A164" t="n">
-        <v>2025</v>
-      </c>
-      <c r="B164" t="n">
-        <v>1</v>
-      </c>
-      <c r="C164" t="n">
-        <v>10</v>
-      </c>
-      <c r="D164" t="inlineStr">
-        <is>
-          <t>Viernes</t>
-        </is>
-      </c>
-      <c r="E164" t="inlineStr">
-        <is>
-          <t>Breinbauer</t>
-        </is>
-      </c>
-      <c r="F164" t="inlineStr">
-        <is>
-          <t>Rubio</t>
-        </is>
-      </c>
-      <c r="G164" t="inlineStr">
-        <is>
-          <t>Recluta1</t>
-        </is>
-      </c>
-      <c r="H164" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> - </t>
-        </is>
-      </c>
-      <c r="I164" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-    </row>
-    <row r="165">
-      <c r="A165" t="n">
-        <v>2025</v>
-      </c>
-      <c r="B165" t="n">
-        <v>1</v>
-      </c>
-      <c r="C165" t="n">
-        <v>11</v>
-      </c>
-      <c r="D165" t="inlineStr">
-        <is>
-          <t>Sábado</t>
-        </is>
-      </c>
-      <c r="E165" t="inlineStr">
-        <is>
-          <t>Recluta1</t>
-        </is>
-      </c>
-      <c r="F165" t="inlineStr">
-        <is>
-          <t>Recluta1</t>
-        </is>
-      </c>
-      <c r="G165" t="inlineStr">
-        <is>
-          <t>Recluta1</t>
-        </is>
-      </c>
-      <c r="H165" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> - </t>
-        </is>
-      </c>
-      <c r="I165" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>

</xml_diff>